<commit_message>
Non degenerate spectrum for 3 qubits
</commit_message>
<xml_diff>
--- a/final_eigenvec_three.xlsx
+++ b/final_eigenvec_three.xlsx
@@ -477,210 +477,210 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6.217406212239571e-21</v>
+        <v>-8.779167981424272e-12</v>
       </c>
       <c r="B2" t="n">
-        <v>-5.275625057681557e-21</v>
+        <v>-1.609528544845711e-11</v>
       </c>
       <c r="C2" t="n">
-        <v>3.219057089704902e-11</v>
+        <v>-9.657171269114809e-11</v>
       </c>
       <c r="D2" t="n">
-        <v>5.275620846622326e-21</v>
+        <v>2.984846159787282e-20</v>
       </c>
       <c r="E2" t="n">
-        <v>2.731461193349775e-11</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>-2.731459451213997e-11</v>
+        <v>6.217560184328447e-22</v>
       </c>
       <c r="G2" t="n">
-        <v>1.931432204919333e-10</v>
+        <v>1.727411654803868e-22</v>
       </c>
       <c r="H2" t="n">
-        <v>-1</v>
+        <v>4.692058802350669e-29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.931437842995357e-10</v>
+        <v>-1.478772354528204e-16</v>
       </c>
       <c r="B3" t="n">
-        <v>3.45647655392911e-16</v>
+        <v>-4.318785482454018e-16</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D3" t="n">
-        <v>-4.901593125158773e-16</v>
+        <v>3.380523074071533e-10</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.365726115649133e-10</v>
+        <v>-9.657171269114488e-11</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.365734379330293e-10</v>
+        <v>-1.9314236368038e-11</v>
       </c>
       <c r="G3" t="n">
-        <v>5.334071672239157e-17</v>
+        <v>-9.656633869885605e-12</v>
       </c>
       <c r="H3" t="n">
-        <v>3.219057089704904e-11</v>
+        <v>1.799092274089556e-19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3.219059206605705e-11</v>
+        <v>-1.154681825411029e-15</v>
       </c>
       <c r="B4" t="n">
-        <v>-2.731460402022783e-11</v>
+        <v>-1</v>
       </c>
       <c r="C4" t="n">
-        <v>2.459222016602375e-17</v>
+        <v>-1.357950826736785e-16</v>
       </c>
       <c r="D4" t="n">
-        <v>2.731460631153943e-11</v>
+        <v>-1.931434253822938e-11</v>
       </c>
       <c r="E4" t="n">
-        <v>1.030076663856088e-16</v>
+        <v>-1.609528544882413e-11</v>
       </c>
       <c r="F4" t="n">
-        <v>-9.760978308568577e-17</v>
+        <v>-5.875310241946868e-17</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>-6.438105270984324e-12</v>
       </c>
       <c r="H4" t="n">
-        <v>1.931435135779936e-10</v>
+        <v>-2.061768773616638e-23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>-6.995381887074578e-17</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-6.437929010255724e-12</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-9.65763618108535e-12</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3.108536132856199e-21</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1.208949519111344e-21</v>
+      </c>
+      <c r="F5" t="n">
+        <v>8.541667303886157e-18</v>
+      </c>
+      <c r="G5" t="n">
         <v>1</v>
       </c>
-      <c r="B5" t="n">
-        <v>1.365730315576971e-10</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-1.931437241363401e-10</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.365730201011393e-10</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2.156604161989864e-16</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2.775036610834975e-17</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-3.219057849715358e-11</v>
-      </c>
       <c r="H5" t="n">
-        <v>-6.217400698932025e-21</v>
+        <v>4.598652985294717e-12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-4.464578364049936e-17</v>
+        <v>-1</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.365730201327928e-10</v>
+        <v>8.405394991419988e-16</v>
       </c>
       <c r="C6" t="n">
-        <v>-4.432244306581715e-16</v>
+        <v>-2.092220421464854e-16</v>
       </c>
       <c r="D6" t="n">
-        <v>1.365730315260431e-10</v>
+        <v>-9.657171269114646e-12</v>
       </c>
       <c r="E6" t="n">
-        <v>0.70710695654703</v>
+        <v>-8.779167983118333e-12</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.7071065052238935</v>
+        <v>-6.438084802858598e-12</v>
       </c>
       <c r="G6" t="n">
-        <v>2.76967488568725e-17</v>
+        <v>-2.547768570861929e-18</v>
       </c>
       <c r="H6" t="n">
-        <v>3.862868507645885e-11</v>
+        <v>-1.612184258303316e-23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-6.806329781980839e-17</v>
+        <v>-6.438114179409815e-12</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.365730315260432e-10</v>
+        <v>3.090924084001512e-27</v>
       </c>
       <c r="C7" t="n">
-        <v>1.931434254926594e-10</v>
+        <v>-1.931461135188511e-11</v>
       </c>
       <c r="D7" t="n">
-        <v>-1.365730201327929e-10</v>
+        <v>6.402104597874661e-21</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7071066058260215</v>
+        <v>-2.543480137108714e-21</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7071070571490938</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>-6.897807984476963e-21</v>
+        <v>1.942890383709254e-16</v>
       </c>
       <c r="H7" t="n">
-        <v>-2.735654737060307e-21</v>
+        <v>3.714296641956536e-12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4.352180292143494e-20</v>
+        <v>-9.657171269114728e-12</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.7071067516922724</v>
+        <v>-1.93143425382294e-11</v>
       </c>
       <c r="C8" t="n">
-        <v>2.317721104587532e-10</v>
+        <v>2.897151380734415e-11</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7071068106808213</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.365730596991424e-10</v>
+        <v>2.40217692243337e-21</v>
       </c>
       <c r="F8" t="n">
-        <v>1.365729725290458e-10</v>
+        <v>5.246550266921314e-23</v>
       </c>
       <c r="G8" t="n">
-        <v>-3.862868507645885e-11</v>
+        <v>1.780216013899641e-23</v>
       </c>
       <c r="H8" t="n">
-        <v>-7.460879960565068e-21</v>
+        <v>3.115111467656421e-12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.931434253822942e-10</v>
+        <v>-3.791118289460318e-23</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.7071068106808214</v>
+        <v>-6.908155685931354e-23</v>
       </c>
       <c r="C9" t="n">
-        <v>-2.984356843292659e-20</v>
+        <v>-8.419587640931153e-19</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.7071067516922726</v>
+        <v>3.115352420863995e-12</v>
       </c>
       <c r="E9" t="n">
-        <v>-1.365729919992527e-10</v>
+        <v>-4.346547728067738e-33</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.365730790902023e-10</v>
+        <v>3.714296641936368e-12</v>
       </c>
       <c r="G9" t="n">
-        <v>4.973915112249691e-21</v>
+        <v>4.598652985297356e-12</v>
       </c>
       <c r="H9" t="n">
-        <v>7.685437548905829e-31</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>